<commit_message>
Tratamento dos valores financeiros da planilha de pagamento
</commit_message>
<xml_diff>
--- a/dados/processados/pagamento_11_jvf.xlsx
+++ b/dados/processados/pagamento_11_jvf.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MAF\Magalhaes\credcom\dados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MAF\Magalhaes\credcom\dados\processados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72E11A3F-1900-45C7-AF08-FC744386A5EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D14F43E-E12C-4CDB-B078-14659DDC29E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A4747583-C4FE-4E55-A275-5BE55944F682}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="280">
   <si>
     <t>Contratante</t>
   </si>
@@ -868,6 +868,18 @@
   </si>
   <si>
     <t>HARMO-164-32-P</t>
+  </si>
+  <si>
+    <t>R$ 440,32</t>
+  </si>
+  <si>
+    <t>R$ 400,29</t>
+  </si>
+  <si>
+    <t>R$ 734,84</t>
+  </si>
+  <si>
+    <t>R$ 668,04</t>
   </si>
 </sst>
 </file>
@@ -1003,7 +1015,21 @@
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1350,8 +1376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D14C30F1-CC51-42FF-9B82-C007E2F8AC9B}">
   <dimension ref="A1:S111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L95" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R119" sqref="R119"/>
+    <sheetView tabSelected="1" topLeftCell="L81" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R93" sqref="R93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6729,8 +6755,8 @@
       <c r="I94" s="8">
         <v>40.03</v>
       </c>
-      <c r="J94" s="8">
-        <v>440.32</v>
+      <c r="J94" s="8" t="s">
+        <v>276</v>
       </c>
       <c r="K94" s="7" t="s">
         <v>240</v>
@@ -6753,8 +6779,8 @@
       <c r="Q94" s="8">
         <v>400.29</v>
       </c>
-      <c r="R94" s="8">
-        <v>400.29</v>
+      <c r="R94" s="8" t="s">
+        <v>277</v>
       </c>
       <c r="S94" s="8"/>
     </row>
@@ -6786,8 +6812,8 @@
       <c r="I95" s="8">
         <v>66.8</v>
       </c>
-      <c r="J95" s="8">
-        <v>734.84</v>
+      <c r="J95" s="8" t="s">
+        <v>278</v>
       </c>
       <c r="K95" s="7" t="s">
         <v>240</v>
@@ -6810,8 +6836,8 @@
       <c r="Q95" s="8">
         <v>668.04</v>
       </c>
-      <c r="R95" s="8">
-        <v>668.04</v>
+      <c r="R95" s="8" t="s">
+        <v>279</v>
       </c>
       <c r="S95" s="8"/>
     </row>
@@ -7733,7 +7759,11 @@
       <sortCondition ref="D1:D111"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="C1:C1048576">
+  <conditionalFormatting sqref="C112:C1048576">
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C111">
     <cfRule type="duplicateValues" dxfId="1" priority="1"/>
     <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>

</xml_diff>